<commit_message>
JNG-3902 Type mapper updated
</commit_message>
<xml_diff>
--- a/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Postgresql.xlsx
+++ b/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Postgresql.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bence/Projects/judo-ng/runtime/judo-tatami-base/judo-tatami-asm2rdbms/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4F6136-0B4B-5B43-BBA2-7EF1CF229629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DEEF6F-29D4-3D43-81C5-2E3875F8C7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21460" yWindow="2400" windowWidth="28000" windowHeight="20180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="4400" windowWidth="28000" windowHeight="20180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
   <dimension ref="A1:G1019"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>